<commit_message>
written final code for search client test
</commit_message>
<xml_diff>
--- a/excelfiles/Demo.xlsx
+++ b/excelfiles/Demo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>TestCase</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Password@12</t>
+  </si>
+  <si>
+    <t>SearchClient</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -230,12 +233,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -245,6 +259,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,6 +676,23 @@
       </c>
       <c r="F7" s="2"/>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -670,9 +702,10 @@
     <hyperlink ref="F5" r:id="rId5"/>
     <hyperlink ref="D6" r:id="rId6"/>
     <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added ssh key and commited
</commit_message>
<xml_diff>
--- a/excelfiles/Demo.xlsx
+++ b/excelfiles/Demo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>TestCase</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>name and email changed</t>
+  </si>
+  <si>
+    <t>SSH Key Added</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,6 +708,11 @@
       </c>
       <c r="B9" s="7" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>